<commit_message>
minor excel issue fixed
</commit_message>
<xml_diff>
--- a/final assignment/data/rfr_strategies.xlsx
+++ b/final assignment/data/rfr_strategies.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhkwakkel/Documents/GitHub/epa1361_open/final assignment/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6922B60-0097-4946-9B09-4CFD3DA8E495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="11700" yWindow="9740" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Olburgen" sheetId="1" r:id="rId1"/>
@@ -68,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,6 +123,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -164,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +206,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,6 +258,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -407,21 +450,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:I1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -440,9 +485,8 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -456,7 +500,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -470,7 +514,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -486,7 +530,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -500,7 +544,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -512,7 +556,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -538,16 +582,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +602,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>903</v>
       </c>
@@ -566,7 +610,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>922</v>
       </c>
@@ -574,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>932</v>
       </c>
@@ -582,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>940</v>
       </c>
@@ -590,7 +634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>947</v>
       </c>
@@ -598,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -612,16 +656,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +676,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>903</v>
       </c>
@@ -641,7 +685,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>922</v>
       </c>
@@ -649,7 +693,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>932</v>
       </c>
@@ -657,7 +701,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>940</v>
       </c>
@@ -665,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>947</v>
       </c>
@@ -673,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -687,16 +731,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +751,7 @@
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>903</v>
       </c>
@@ -716,7 +760,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>922</v>
       </c>
@@ -724,7 +768,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>932</v>
       </c>
@@ -732,7 +776,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>940</v>
       </c>
@@ -740,7 +784,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>947</v>
       </c>
@@ -748,7 +792,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -762,19 +806,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +829,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>903</v>
       </c>
@@ -794,7 +838,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>922</v>
       </c>
@@ -802,7 +846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>932</v>
       </c>
@@ -810,7 +854,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>940</v>
       </c>
@@ -818,7 +862,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>947</v>
       </c>
@@ -826,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>

</xml_diff>